<commit_message>
Add generateSQL to create table
</commit_message>
<xml_diff>
--- a/sampleFile/catapult.xlsx
+++ b/sampleFile/catapult.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" state="visible" r:id="rId2"/>
@@ -192,6 +192,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -202,6 +203,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -228,6 +230,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -238,6 +241,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -264,6 +268,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -274,6 +279,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">rd</t>
     </r>
@@ -300,6 +306,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -310,6 +317,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -336,6 +344,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -346,6 +355,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -369,7 +379,7 @@
     <t xml:space="preserve">T#ApplicantName</t>
   </si>
   <si>
-    <t xml:space="preserve">ApplicantName</t>
+    <t xml:space="preserve">Applicant Name</t>
   </si>
   <si>
     <t xml:space="preserve">Y#Consent</t>
@@ -380,6 +390,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Consent of share information tho 3</t>
     </r>
@@ -389,6 +400,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">rd</t>
     </r>
@@ -397,6 +409,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Party</t>
     </r>
@@ -427,6 +440,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -449,18 +463,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -468,12 +485,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -639,11 +658,11 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
@@ -804,7 +823,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1146,11 +1165,11 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="27.23"/>

</xml_diff>